<commit_message>
Lamp item and balancing
</commit_message>
<xml_diff>
--- a/StructureLocs.xlsx
+++ b/StructureLocs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\mctradepost-retro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F85D5A-B2A4-4FC3-A21E-6EB6FB32AD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4CD0FCE-8A01-49CF-9B2E-4FAA1568F674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7350" yWindow="1080" windowWidth="31650" windowHeight="18540" xr2:uid="{A8250FA9-3FEF-4870-A5B5-D9F655C06814}"/>
+    <workbookView xWindow="12465" yWindow="840" windowWidth="23580" windowHeight="18540" xr2:uid="{A8250FA9-3FEF-4870-A5B5-D9F655C06814}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="98">
   <si>
     <t>Building</t>
   </si>
@@ -297,6 +297,39 @@
   </si>
   <si>
     <t>2488 -35 -191</t>
+  </si>
+  <si>
+    <t>university</t>
+  </si>
+  <si>
+    <t>1480 -51 1</t>
+  </si>
+  <si>
+    <t>1508 -30 -36</t>
+  </si>
+  <si>
+    <t>1480 -51 -47</t>
+  </si>
+  <si>
+    <t>1508 -30 -84</t>
+  </si>
+  <si>
+    <t>1480 -51 -95</t>
+  </si>
+  <si>
+    <t>1508 -30 -132</t>
+  </si>
+  <si>
+    <t>1480 -51 -143</t>
+  </si>
+  <si>
+    <t>1508 -30 -180</t>
+  </si>
+  <si>
+    <t>1480 -51 -191</t>
+  </si>
+  <si>
+    <t>1508 -30 -228</t>
   </si>
 </sst>
 </file>
@@ -671,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B118C272-02CF-4264-9B2B-F749CC7F7D83}">
   <dimension ref="A1:E141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1856,48 +1889,93 @@
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>87</v>
+      </c>
       <c r="B97">
         <v>1</v>
       </c>
+      <c r="C97" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="E97" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>/structurize scan 1480 -51 1 1508 -30 -36 @p "trade post/economic/university1"</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>87</v>
+      </c>
       <c r="B98">
         <v>2</v>
       </c>
+      <c r="C98" t="s">
+        <v>90</v>
+      </c>
+      <c r="D98" t="s">
+        <v>91</v>
+      </c>
       <c r="E98" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>/structurize scan 1480 -51 -47 1508 -30 -84 @p "trade post/economic/university2"</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>87</v>
+      </c>
       <c r="B99">
         <v>3</v>
       </c>
+      <c r="C99" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D99" t="s">
+        <v>93</v>
+      </c>
       <c r="E99" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>/structurize scan 1480 -51 -95 1508 -30 -132 @p "trade post/economic/university3"</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>87</v>
+      </c>
       <c r="B100">
         <v>4</v>
       </c>
+      <c r="C100" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="E100" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>/structurize scan 1480 -51 -143 1508 -30 -180 @p "trade post/economic/university4"</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>87</v>
+      </c>
       <c r="B101">
         <v>5</v>
       </c>
+      <c r="C101" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="E101" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>/structurize scan 1480 -51 -191 1508 -30 -228 @p "trade post/economic/university5"</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>